<commit_message>
Se implementan estilos en la interfaz del slider
</commit_message>
<xml_diff>
--- a/service/Resources/Base-expo-estudiantes.xlsx
+++ b/service/Resources/Base-expo-estudiantes.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\appexpoestudiantes\service\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="The export" sheetId="1" r:id="rId1"/>
+    <sheet name="The export" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>User Name</t>
   </si>
@@ -63,68 +59,49 @@
     <t>Cier</t>
   </si>
   <si>
+    <t>Chapinero</t>
+  </si>
+  <si>
+    <t>Tecnología</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>https://www.nestforms.com/files/uploaded_files/e354136/event_354136_13.jpg</t>
+  </si>
+  <si>
     <t>Usaquén</t>
   </si>
   <si>
-    <t>Matemáticas</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>https://www.nestforms.com/files/uploaded_files/e353738/event_353738_7.jpg</t>
-  </si>
-  <si>
-    <t>San Cristóbal</t>
-  </si>
-  <si>
-    <t>Ingeniería</t>
-  </si>
-  <si>
-    <t>https://www.nestforms.com/files/uploaded_files/e353729/event_353729_6.jpg</t>
-  </si>
-  <si>
-    <t>Santa Fe</t>
-  </si>
-  <si>
     <t>Ciencias</t>
   </si>
   <si>
-    <t>https://www.nestforms.com/files/uploaded_files/e353706/event_353706_5.jpg</t>
-  </si>
-  <si>
-    <t>Chapinero</t>
-  </si>
-  <si>
-    <t>Tecnología</t>
-  </si>
-  <si>
-    <t>https://www.nestforms.com/files/uploaded_files/e353702/event_353702_4.jpg</t>
-  </si>
-  <si>
-    <t>https://www.nestforms.com/files/uploaded_files/e353699/event_353699_3.jpg</t>
+    <t>https://www.nestforms.com/files/uploaded_files/e354135/event_354135_12.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -133,41 +110,31 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="2">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -457,32 +424,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="88.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="114.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="83.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="87.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="26.993408" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="88.406982" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="80.12329099999999" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="114.257813" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="83.693848" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="88.406982" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -534,16 +504,16 @@
         <v>15</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -569,89 +539,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-  </hyperlinks>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>